<commit_message>
Updated imputation procedure, first steps of imputed case analysis
</commit_message>
<xml_diff>
--- a/Analysis/Comp_comb_plant.xlsx
+++ b/Analysis/Comp_comb_plant.xlsx
@@ -515,7 +515,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cattle</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cattle</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -930,7 +930,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Cattle</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Cattle</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ungulates</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Beaver</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Beaver</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Beaver</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Beaver</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3060,7 +3060,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3070,7 +3070,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3568,7 +3568,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3900,7 +3900,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -4195,19 +4195,19 @@
         <v>64</v>
       </c>
       <c r="O46">
-        <v>66.02910602910603</v>
+        <v>0.6645915469470783</v>
       </c>
       <c r="P46">
-        <v>19.95841995841999</v>
+        <v>2.456123440944749</v>
       </c>
       <c r="Q46">
         <v>64</v>
       </c>
       <c r="R46">
-        <v>25.44698544698545</v>
+        <v>-1.074913191092807</v>
       </c>
       <c r="S46">
-        <v>25.28066528066529</v>
+        <v>5.011375609674042</v>
       </c>
       <c r="T46" t="inlineStr">
         <is>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -4295,19 +4295,19 @@
         <v>64</v>
       </c>
       <c r="O47">
-        <v>66.02910602910603</v>
+        <v>0.6645915469470783</v>
       </c>
       <c r="P47">
-        <v>19.95841995841999</v>
+        <v>2.456123440944749</v>
       </c>
       <c r="Q47">
         <v>64</v>
       </c>
       <c r="R47">
-        <v>17.29729729729731</v>
+        <v>-1.564702018592708</v>
       </c>
       <c r="S47">
-        <v>22.61954261954262</v>
+        <v>5.438386561619762</v>
       </c>
       <c r="T47" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -4395,19 +4395,19 @@
         <v>64</v>
       </c>
       <c r="O48">
-        <v>66.02910602910603</v>
+        <v>0.6645915469470783</v>
       </c>
       <c r="P48">
-        <v>19.95841995841999</v>
+        <v>2.456123440944749</v>
       </c>
       <c r="Q48">
         <v>64</v>
       </c>
       <c r="R48">
-        <v>9.480249480249491</v>
+        <v>-2.256357432280105</v>
       </c>
       <c r="S48">
-        <v>17.29729729729729</v>
+        <v>5.616825552931346</v>
       </c>
       <c r="T48" t="inlineStr">
         <is>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -4495,19 +4495,19 @@
         <v>64</v>
       </c>
       <c r="O49">
-        <v>72.34927234927235</v>
+        <v>0.9618533515527208</v>
       </c>
       <c r="P49">
-        <v>19.95841995841988</v>
+        <v>2.346397226232656</v>
       </c>
       <c r="Q49">
         <v>64</v>
       </c>
       <c r="R49">
-        <v>19.2931392931393</v>
+        <v>-1.431074030942754</v>
       </c>
       <c r="S49">
-        <v>25.28066528066529</v>
+        <v>5.755318862234189</v>
       </c>
       <c r="T49" t="inlineStr">
         <is>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -4595,19 +4595,19 @@
         <v>64</v>
       </c>
       <c r="O50">
-        <v>72.34927234927235</v>
+        <v>0.9618533515527208</v>
       </c>
       <c r="P50">
-        <v>19.95841995841988</v>
+        <v>2.346397226232656</v>
       </c>
       <c r="Q50">
         <v>64</v>
       </c>
       <c r="R50">
-        <v>11.30977130977132</v>
+        <v>-2.059482652175352</v>
       </c>
       <c r="S50">
-        <v>22.61954261954264</v>
+        <v>6.725414908905554</v>
       </c>
       <c r="T50" t="inlineStr">
         <is>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -4695,19 +4695,19 @@
         <v>64</v>
       </c>
       <c r="O51">
-        <v>72.34927234927235</v>
+        <v>0.9618533515527208</v>
       </c>
       <c r="P51">
-        <v>19.95841995841988</v>
+        <v>2.346397226232656</v>
       </c>
       <c r="Q51">
         <v>64</v>
       </c>
       <c r="R51">
-        <v>58.71101871101871</v>
+        <v>0.352031754008015</v>
       </c>
       <c r="S51">
-        <v>19.95841995841999</v>
+        <v>2.604696105940015</v>
       </c>
       <c r="T51" t="inlineStr">
         <is>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -4749,7 +4749,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -4795,19 +4795,19 @@
         <v>48</v>
       </c>
       <c r="O52">
-        <v>57.19063545150499</v>
+        <v>0.2896332925830415</v>
       </c>
       <c r="P52">
-        <v>76.46511926391041</v>
+        <v>10.11114316401136</v>
       </c>
       <c r="Q52">
         <v>48</v>
       </c>
       <c r="R52">
-        <v>20.73578595317726</v>
+        <v>-1.340925756090039</v>
       </c>
       <c r="S52">
-        <v>71.83086961155217</v>
+        <v>15.77425434967047</v>
       </c>
       <c r="T52" t="inlineStr">
         <is>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4895,19 +4895,19 @@
         <v>90</v>
       </c>
       <c r="O53">
-        <v>58.76923076923077</v>
+        <v>0.3544336280957182</v>
       </c>
       <c r="P53">
-        <v>93.40881703881976</v>
+        <v>12.18463279010214</v>
       </c>
       <c r="Q53">
         <v>90</v>
       </c>
       <c r="R53">
-        <v>20.00000000000003</v>
+        <v>-1.386294361119889</v>
       </c>
       <c r="S53">
-        <v>93.40881703881976</v>
+        <v>20.88678646331025</v>
       </c>
       <c r="T53" t="inlineStr">
         <is>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4995,19 +4995,19 @@
         <v>48</v>
       </c>
       <c r="O54">
-        <v>59.5808383233533</v>
+        <v>0.3880300462860632</v>
       </c>
       <c r="P54">
-        <v>64.30368267620986</v>
+        <v>8.330703146777585</v>
       </c>
       <c r="Q54">
         <v>48</v>
       </c>
       <c r="R54">
-        <v>20.35928143712577</v>
+        <v>-1.363988603605591</v>
       </c>
       <c r="S54">
-        <v>64.30368267620976</v>
+        <v>14.25121975864779</v>
       </c>
       <c r="T54" t="inlineStr">
         <is>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -5095,19 +5095,19 @@
         <v>90</v>
       </c>
       <c r="O55">
-        <v>70.07042253521131</v>
+        <v>0.8506535682341779</v>
       </c>
       <c r="P55">
-        <v>66.80868296130372</v>
+        <v>7.981138506182281</v>
       </c>
       <c r="Q55">
         <v>90</v>
       </c>
       <c r="R55">
-        <v>4.929577464788792</v>
+        <v>-2.959364629383103</v>
       </c>
       <c r="S55">
-        <v>66.80868296130386</v>
+        <v>30.08969389127185</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -5195,19 +5195,19 @@
         <v>48</v>
       </c>
       <c r="O56">
-        <v>78.988326848249</v>
+        <v>1.324221932477512</v>
       </c>
       <c r="P56">
-        <v>40.436983834293</v>
+        <v>4.549834668506687</v>
       </c>
       <c r="Q56">
         <v>48</v>
       </c>
       <c r="R56">
-        <v>2.33463035019453</v>
+        <v>-3.733693469903739</v>
       </c>
       <c r="S56">
-        <v>35.04538598972054</v>
+        <v>22.93131799524272</v>
       </c>
       <c r="T56" t="inlineStr">
         <is>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -5295,19 +5295,19 @@
         <v>90</v>
       </c>
       <c r="O57">
-        <v>29.23588039867109</v>
+        <v>-0.8839553512312189</v>
       </c>
       <c r="P57">
-        <v>53.58011982345104</v>
+        <v>9.90930057676136</v>
       </c>
       <c r="Q57">
         <v>90</v>
       </c>
       <c r="R57">
-        <v>44.18604651162789</v>
+        <v>-0.2336148511815058</v>
       </c>
       <c r="S57">
-        <v>47.27657631480956</v>
+        <v>7.112155534885336</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -5349,7 +5349,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -5395,19 +5395,19 @@
         <v>6</v>
       </c>
       <c r="O58">
-        <v>54.84949832775919</v>
+        <v>0.1945916493857688</v>
       </c>
       <c r="P58">
-        <v>32.76909354893883</v>
+        <v>4.424604026796255</v>
       </c>
       <c r="Q58">
         <v>6</v>
       </c>
       <c r="R58">
-        <v>25.75250836120402</v>
+        <v>-1.058871960018595</v>
       </c>
       <c r="S58">
-        <v>32.76909354893883</v>
+        <v>6.457238021401541</v>
       </c>
       <c r="T58" t="inlineStr">
         <is>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -5495,19 +5495,19 @@
         <v>6</v>
       </c>
       <c r="O59">
-        <v>54.49101796407187</v>
+        <v>0.1801261662305197</v>
       </c>
       <c r="P59">
-        <v>25.66830568784768</v>
+        <v>3.477192159559847</v>
       </c>
       <c r="Q59">
         <v>6</v>
       </c>
       <c r="R59">
-        <v>22.75449101796409</v>
+        <v>-1.222226244635286</v>
       </c>
       <c r="S59">
-        <v>27.86844617537746</v>
+        <v>5.842071671790914</v>
       </c>
       <c r="T59" t="inlineStr">
         <is>
@@ -5539,7 +5539,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -5595,19 +5595,19 @@
         <v>6</v>
       </c>
       <c r="O60">
-        <v>53.53846153846155</v>
+        <v>0.141775462399605</v>
       </c>
       <c r="P60">
-        <v>27.13280945852139</v>
+        <v>3.708141601196324</v>
       </c>
       <c r="Q60">
         <v>6</v>
       </c>
       <c r="R60">
-        <v>23.07692307692311</v>
+        <v>-1.203972804325934</v>
       </c>
       <c r="S60">
-        <v>24.87174200364452</v>
+        <v>5.177284281908125</v>
       </c>
       <c r="T60" t="inlineStr">
         <is>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -5649,7 +5649,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -5695,19 +5695,19 @@
         <v>6</v>
       </c>
       <c r="O61">
-        <v>75.87548638132294</v>
+        <v>1.145865173518654</v>
       </c>
       <c r="P61">
-        <v>22.87461238396741</v>
+        <v>2.626016974719664</v>
       </c>
       <c r="Q61">
         <v>6</v>
       </c>
       <c r="R61">
-        <v>5.058365758754846</v>
+        <v>-2.932218867831669</v>
       </c>
       <c r="S61">
-        <v>22.87461238396744</v>
+        <v>10.16864845566765</v>
       </c>
       <c r="T61" t="inlineStr">
         <is>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -5749,7 +5749,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -5795,19 +5795,19 @@
         <v>6</v>
       </c>
       <c r="O62">
-        <v>98.59154929577467</v>
+        <v>4.248495242049376</v>
       </c>
       <c r="P62">
-        <v>17.2499277660787</v>
+        <v>1.737240847946985</v>
       </c>
       <c r="Q62">
         <v>6</v>
       </c>
       <c r="R62">
-        <v>61.61971830985918</v>
+        <v>0.4734380916943716</v>
       </c>
       <c r="S62">
-        <v>15.52493498947091</v>
+        <v>1.977676762508595</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -5839,7 +5839,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -5895,19 +5895,19 @@
         <v>6</v>
       </c>
       <c r="O63">
-        <v>81.39534883720928</v>
+        <v>1.475906519809576</v>
       </c>
       <c r="P63">
-        <v>17.08946332174311</v>
+        <v>1.894172353707069</v>
       </c>
       <c r="Q63">
         <v>6</v>
       </c>
       <c r="R63">
-        <v>97.34219269102989</v>
+        <v>3.600731067337229</v>
       </c>
       <c r="S63">
-        <v>13.0205434832328</v>
+        <v>1.319670139537233</v>
       </c>
       <c r="T63" t="inlineStr">
         <is>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -5949,7 +5949,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -5995,19 +5995,19 @@
         <v>6</v>
       </c>
       <c r="O64">
-        <v>86.82634730538922</v>
+        <v>1.885691289062258</v>
       </c>
       <c r="P64">
-        <v>24.20154536282784</v>
+        <v>2.597245857243066</v>
       </c>
       <c r="Q64">
         <v>6</v>
       </c>
       <c r="R64">
-        <v>52.69461077844312</v>
+        <v>0.1078889620111851</v>
       </c>
       <c r="S64">
-        <v>24.93492552533773</v>
+        <v>3.434933587141446</v>
       </c>
       <c r="T64" t="inlineStr">
         <is>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -6095,19 +6095,19 @@
         <v>6</v>
       </c>
       <c r="O65">
-        <v>86.76923076923077</v>
+        <v>1.880706955244552</v>
       </c>
       <c r="P65">
-        <v>23.36436370039334</v>
+        <v>2.508225041019831</v>
       </c>
       <c r="Q65">
         <v>6</v>
       </c>
       <c r="R65">
-        <v>52.61538461538464</v>
+        <v>0.1047109540890318</v>
       </c>
       <c r="S65">
-        <v>24.87174200364452</v>
+        <v>3.428807907634629</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -6195,19 +6195,19 @@
         <v>6</v>
       </c>
       <c r="O66">
-        <v>93.97993311036788</v>
+        <v>2.74798291143758</v>
       </c>
       <c r="P66">
-        <v>19.66145612936327</v>
+        <v>2.028112935206314</v>
       </c>
       <c r="Q66">
         <v>6</v>
       </c>
       <c r="R66">
-        <v>50.83612040133778</v>
+        <v>0.03344793406753969</v>
       </c>
       <c r="S66">
-        <v>18.8422287906398</v>
+        <v>2.642615857046959</v>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -6249,7 +6249,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Pademelon (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -6295,19 +6295,19 @@
         <v>6</v>
       </c>
       <c r="O67">
-        <v>98.05447470817118</v>
+        <v>3.919991175077309</v>
       </c>
       <c r="P67">
-        <v>6.671761945323841</v>
+        <v>0.6736852996662777</v>
       </c>
       <c r="Q67">
         <v>6</v>
       </c>
       <c r="R67">
-        <v>14.78599221789881</v>
+        <v>-1.751485570090117</v>
       </c>
       <c r="S67">
-        <v>8.577979643987788</v>
+        <v>2.229765426227599</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -6339,7 +6339,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Possum (captive)</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6395,19 +6395,19 @@
         <v>6</v>
       </c>
       <c r="O68">
-        <v>89.03654485049832</v>
+        <v>2.094479419044374</v>
       </c>
       <c r="P68">
-        <v>8.137839677020624</v>
+        <v>0.8623590898619642</v>
       </c>
       <c r="Q68">
         <v>6</v>
       </c>
       <c r="R68">
-        <v>98.67109634551493</v>
+        <v>4.307437777682794</v>
       </c>
       <c r="S68">
-        <v>6.510271741616472</v>
+        <v>0.6553181618869695</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -6495,19 +6495,19 @@
         <v>96</v>
       </c>
       <c r="O69">
-        <v>61.87713310580203</v>
+        <v>0.4843364116856495</v>
       </c>
       <c r="P69">
-        <v>28.08971172611414</v>
+        <v>3.570900437363647</v>
       </c>
       <c r="Q69">
         <v>23</v>
       </c>
       <c r="R69">
-        <v>46.82593856655288</v>
+        <v>-0.1271334181448639</v>
       </c>
       <c r="S69">
-        <v>36.66437751611089</v>
+        <v>5.357937202821788</v>
       </c>
       <c r="T69" t="inlineStr">
         <is>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -6595,19 +6595,19 @@
         <v>108</v>
       </c>
       <c r="O70">
-        <v>55.62347188264058</v>
+        <v>0.2258945846860995</v>
       </c>
       <c r="P70">
-        <v>39.12994978468565</v>
+        <v>5.246596843224606</v>
       </c>
       <c r="Q70">
         <v>55</v>
       </c>
       <c r="R70">
-        <v>42.78728606356967</v>
+        <v>-0.2905351414341878</v>
       </c>
       <c r="S70">
-        <v>35.53972869121642</v>
+        <v>5.433162787804286</v>
       </c>
       <c r="T70" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -6695,19 +6695,19 @@
         <v>4</v>
       </c>
       <c r="O71">
-        <v>0.3481751824817519</v>
+        <v>-0.6270700899881577</v>
       </c>
       <c r="P71">
-        <v>0.1138686131386861</v>
+        <v>1.084061345602135</v>
       </c>
       <c r="Q71">
         <v>4</v>
       </c>
       <c r="R71">
-        <v>0.221167883211679</v>
+        <v>-1.258873445792383</v>
       </c>
       <c r="S71">
-        <v>0.1007299270072994</v>
+        <v>1.04752469561917</v>
       </c>
       <c r="T71" t="inlineStr">
         <is>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -6795,19 +6795,19 @@
         <v>4</v>
       </c>
       <c r="O72">
-        <v>0.3766423357664234</v>
+        <v>-0.5038244283070068</v>
       </c>
       <c r="P72">
-        <v>0.127007299270073</v>
+        <v>1.099153454338057</v>
       </c>
       <c r="Q72">
         <v>4</v>
       </c>
       <c r="R72">
-        <v>0.1708029197080294</v>
+        <v>-1.579947483923394</v>
       </c>
       <c r="S72">
-        <v>0.1007299270072992</v>
+        <v>1.04376967914519</v>
       </c>
       <c r="T72" t="inlineStr">
         <is>
@@ -6839,7 +6839,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -6895,19 +6895,19 @@
         <v>4</v>
       </c>
       <c r="O73">
-        <v>0.3635036496350367</v>
+        <v>-0.560189346884326</v>
       </c>
       <c r="P73">
-        <v>0.1138686131386861</v>
+        <v>1.08991857504101</v>
       </c>
       <c r="Q73">
         <v>4</v>
       </c>
       <c r="R73">
-        <v>0.1927007299270074</v>
+        <v>-1.432556078935963</v>
       </c>
       <c r="S73">
-        <v>0.09635036496350358</v>
+        <v>1.042468625030766</v>
       </c>
       <c r="T73" t="inlineStr">
         <is>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -6949,7 +6949,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -6995,19 +6995,19 @@
         <v>4</v>
       </c>
       <c r="O74">
-        <v>0.3457249070631969</v>
+        <v>-0.6378845018848964</v>
       </c>
       <c r="P74">
-        <v>0.1159851301115244</v>
+        <v>1.083818549022401</v>
       </c>
       <c r="Q74">
         <v>4</v>
       </c>
       <c r="R74">
-        <v>0.1137546468401489</v>
+        <v>-2.052949926232858</v>
       </c>
       <c r="S74">
-        <v>0.07583643122676564</v>
+        <v>1.031342514579477</v>
       </c>
       <c r="T74" t="inlineStr">
         <is>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -7095,19 +7095,19 @@
         <v>4</v>
       </c>
       <c r="O75">
-        <v>0.5040892193308548</v>
+        <v>0.01635724202477102</v>
       </c>
       <c r="P75">
-        <v>0.1249070631970262</v>
+        <v>1.171163262864323</v>
       </c>
       <c r="Q75">
         <v>4</v>
       </c>
       <c r="R75">
-        <v>0.03345724907063219</v>
+        <v>-3.363457053679302</v>
       </c>
       <c r="S75">
-        <v>0.04460966542750922</v>
+        <v>1.029854453722139</v>
       </c>
       <c r="T75" t="inlineStr">
         <is>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -7149,7 +7149,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -7195,19 +7195,19 @@
         <v>4</v>
       </c>
       <c r="O76">
-        <v>0.3301115241635688</v>
+        <v>-0.707680695176113</v>
       </c>
       <c r="P76">
-        <v>0.115985130111524</v>
+        <v>1.07844923740431</v>
       </c>
       <c r="Q76">
         <v>4</v>
       </c>
       <c r="R76">
-        <v>0.03345724907063219</v>
+        <v>-3.363457053679302</v>
       </c>
       <c r="S76">
-        <v>0.04460966542750922</v>
+        <v>1.029854453722139</v>
       </c>
       <c r="T76" t="inlineStr">
         <is>
@@ -7239,7 +7239,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -7249,7 +7249,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -7295,19 +7295,19 @@
         <v>5</v>
       </c>
       <c r="O77">
-        <v>0.4934426229508198</v>
+        <v>-0.0262310121488693</v>
       </c>
       <c r="P77">
-        <v>0.1218840331997836</v>
+        <v>1.162737379669453</v>
       </c>
       <c r="Q77">
         <v>5</v>
       </c>
       <c r="R77">
-        <v>0.4848360655737705</v>
+        <v>-0.06067434461186064</v>
       </c>
       <c r="S77">
-        <v>0.1154690840840056</v>
+        <v>1.155336569909553</v>
       </c>
       <c r="T77" t="inlineStr">
         <is>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Moose</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -7395,19 +7395,19 @@
         <v>5</v>
       </c>
       <c r="O78">
-        <v>0.4934426229508198</v>
+        <v>-0.0262310121488693</v>
       </c>
       <c r="P78">
-        <v>0.1218840331997836</v>
+        <v>1.162737379669453</v>
       </c>
       <c r="Q78">
         <v>5</v>
       </c>
       <c r="R78">
-        <v>0.1032786885245903</v>
+        <v>-2.161314076030447</v>
       </c>
       <c r="S78">
-        <v>0.06414949115778056</v>
+        <v>1.025000810318442</v>
       </c>
       <c r="T78" t="inlineStr">
         <is>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Repellent (absorption)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -7449,7 +7449,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -7516,7 +7516,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -7526,7 +7526,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -7593,7 +7593,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -7670,7 +7670,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -7680,7 +7680,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -7747,7 +7747,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -7757,7 +7757,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -7834,7 +7834,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Rabbits</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -7901,7 +7901,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -7911,7 +7911,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -7978,7 +7978,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -8055,7 +8055,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -8132,7 +8132,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -8142,7 +8142,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -8209,7 +8209,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -8219,7 +8219,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -8286,7 +8286,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -8363,7 +8363,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -8373,7 +8373,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -8440,7 +8440,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -8450,7 +8450,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -8517,7 +8517,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -8527,7 +8527,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -8594,7 +8594,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -8604,7 +8604,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -8681,7 +8681,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -8758,7 +8758,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -8825,7 +8825,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -8835,7 +8835,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -8902,7 +8902,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -8912,7 +8912,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -8979,7 +8979,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -9056,7 +9056,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -9066,7 +9066,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -9133,7 +9133,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -9143,7 +9143,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -9210,7 +9210,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -9220,7 +9220,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -9287,7 +9287,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -9297,7 +9297,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -9364,7 +9364,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -9374,7 +9374,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -9441,7 +9441,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -9451,7 +9451,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -9518,7 +9518,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -9528,7 +9528,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -9605,7 +9605,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -9672,7 +9672,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -9682,7 +9682,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -9749,7 +9749,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -9759,7 +9759,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -9826,7 +9826,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -9836,7 +9836,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -9903,7 +9903,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -9913,7 +9913,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -9980,7 +9980,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -9990,7 +9990,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -10057,7 +10057,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -10067,7 +10067,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -10134,7 +10134,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -10211,7 +10211,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -10288,7 +10288,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -10298,7 +10298,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -10365,7 +10365,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -10375,7 +10375,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -10442,7 +10442,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -10452,7 +10452,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -10519,7 +10519,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -10596,7 +10596,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -10606,7 +10606,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -10673,7 +10673,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -10683,7 +10683,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -10750,7 +10750,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -10760,7 +10760,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -10827,7 +10827,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -10837,7 +10837,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -10904,7 +10904,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -10914,7 +10914,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Repellent (on ground)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -11058,7 +11058,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -11068,7 +11068,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -11135,7 +11135,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -11145,7 +11145,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -11212,7 +11212,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -11222,7 +11222,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -11289,7 +11289,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -11299,7 +11299,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -11376,7 +11376,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Hares</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -11443,7 +11443,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -11453,7 +11453,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -11520,7 +11520,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -11530,7 +11530,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -11597,7 +11597,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -11607,7 +11607,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -11674,7 +11674,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -11684,7 +11684,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -11751,7 +11751,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -11761,7 +11761,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -11828,7 +11828,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -11838,7 +11838,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -11915,7 +11915,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -11982,7 +11982,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -11992,7 +11992,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -12059,7 +12059,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -12069,7 +12069,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -12136,7 +12136,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -12146,7 +12146,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -12213,7 +12213,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -12223,7 +12223,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -12290,7 +12290,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -12300,7 +12300,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -12367,7 +12367,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -12377,7 +12377,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -12444,7 +12444,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -12454,7 +12454,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -12521,7 +12521,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -12531,7 +12531,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -12608,7 +12608,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -12675,7 +12675,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -12685,7 +12685,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -12752,7 +12752,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Repellent (on-browse)</t>
+          <t>Repellents</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -12762,7 +12762,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Goats</t>
+          <t>Other ungulates</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">

</xml_diff>